<commit_message>
Change example and remove some ssl mess
Don't need to change ssl for urls that already have a full path.
</commit_message>
<xml_diff>
--- a/Check-URL-Redirects/Inputs/Example.xlsx
+++ b/Check-URL-Redirects/Inputs/Example.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferguson/Documents/ML-SentrySafe/master-lock-seo-scripts/Check-URL-Redirects/Redirect-Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rferguson/Documents/automated-testing/Check-URL-Redirects/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="1200" yWindow="1300" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Redirects" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,26 +27,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>  www.masterlock.com/index.jsp</t>
   </si>
   <si>
-    <t>http://www.masterlock.com</t>
-  </si>
-  <si>
     <t>  www.masterlock.com/service-and-support/faqs/lostcombo.shtml</t>
   </si>
   <si>
-    <t>http://www.masterlock.comz</t>
-  </si>
-  <si>
     <t>  www.masterlock.com/apps/masterlock/catalog/consumer_product.jsp?sub_cat_id=MLGROUP_1500ID</t>
   </si>
   <si>
-    <t>http://www.masterlock.com/cms/customersupport/current-pricing</t>
-  </si>
-  <si>
     <t>  www.masterlock.com/apps/utilities/img.jsp?i=MLCOM_PRODUCT_5900D.jpg&amp;w=285&amp;u=1&amp;cs=1&amp;t=p</t>
   </si>
   <si>
@@ -62,9 +53,6 @@
     <t>  www.masterlock.com/general/faqs_lostcom.shtml</t>
   </si>
   <si>
-    <t>http://www.masterlock.com/service-and-support/faqs/lost-combinations</t>
-  </si>
-  <si>
     <t>  www.masterlock.com/government/apps/nsn/detail.jsp?nsn=5340-00-158-3807</t>
   </si>
   <si>
@@ -113,61 +101,50 @@
     <t>  www.masterlock.com/business-use/product/175DLH</t>
   </si>
   <si>
-    <t>http://www.masterlock.com/personal-use/product/175DLH</t>
-  </si>
-  <si>
     <t>  www.masterlock.com/business-use/safety-solutions/products/index.jsp?id=27892</t>
   </si>
   <si>
-    <t>http://www.masterlock.com/business-use/product-search/safety-solutions</t>
-  </si>
-  <si>
     <t>  www.masterlock.com/construction%3EMasterlock%3C/a%3E%3C/h2%3E%3Ch3%3E%3Ca%20href=</t>
   </si>
   <si>
-    <t>http://www.masterlock.com/business-use/commercial-security</t>
-  </si>
-  <si>
     <t>  www.masterlock.com/general/Legal.html</t>
   </si>
   <si>
-    <t>http://www.masterlock.com/legal-statement</t>
-  </si>
-  <si>
     <t>URL that needs to be Redirected</t>
   </si>
   <si>
     <t>URL to redirect to</t>
+  </si>
+  <si>
+    <t>https://www.masterlock.com</t>
+  </si>
+  <si>
+    <t>https://www.masterlock.comz</t>
+  </si>
+  <si>
+    <t>https://www.masterlock.com/cms/customersupport/current-pricing</t>
+  </si>
+  <si>
+    <t>https://www.masterlock.com/personal-use/product/175DLH</t>
+  </si>
+  <si>
+    <t>https://www.masterlock.com/business-use/product-search/safety-solutions</t>
+  </si>
+  <si>
+    <t>https://www.masterlock.com/business-use/commercial-security</t>
+  </si>
+  <si>
+    <t>https://www.masterlock.com/legal-statement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,22 +158,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -208,21 +175,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -501,7 +461,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,158 +471,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>36</v>
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B15" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>32</v>
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="B13" r:id="rId5"/>
+    <hyperlink ref="B16" r:id="rId6"/>
+    <hyperlink ref="B17" r:id="rId7"/>
+    <hyperlink ref="B18" r:id="rId8"/>
+    <hyperlink ref="B19" r:id="rId9"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>